<commit_message>
adding the diagram files in the diagram folder
</commit_message>
<xml_diff>
--- a/data/questions_and_choices.xlsx
+++ b/data/questions_and_choices.xlsx
@@ -20,7 +20,31 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+  <si>
+    <t xml:space="preserve">NO.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">questions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">choice1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">choice2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">choice3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">choice4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">answer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">image</t>
+  </si>
   <si>
     <t xml:space="preserve">خوب هستید؟</t>
   </si>
@@ -35,6 +59,9 @@
   </si>
   <si>
     <t xml:space="preserve">no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">none</t>
   </si>
   <si>
     <t xml:space="preserve">چی کارا میکنی؟</t>
@@ -154,10 +181,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -166,13 +193,13 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="0" t="s">
@@ -181,22 +208,66 @@
       <c r="E1" s="0" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>5</v>
+      <c r="A2" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>